<commit_message>
QA -Table 1-3 finished
</commit_message>
<xml_diff>
--- a/QA/Big_Omega_Project-Test Table.xlsx
+++ b/QA/Big_Omega_Project-Test Table.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ME\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FD511E-652A-4891-BB3A-A619214D0551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D234DCE-38BD-4DED-BF0F-A7E6915F99F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B391B523-F954-4CD5-9C14-21981E3766E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B391B523-F954-4CD5-9C14-21981E3766E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист3" sheetId="3" r:id="rId2"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="to">Лист1!$M$9</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="55">
   <si>
     <t xml:space="preserve">Test Case ID        </t>
   </si>
@@ -173,6 +174,36 @@
   </si>
   <si>
     <t>";</t>
+  </si>
+  <si>
+    <t>Function 3</t>
+  </si>
+  <si>
+    <t>3;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                 +;</t>
+  </si>
+  <si>
+    <t>113;</t>
+  </si>
+  <si>
+    <t>4;</t>
+  </si>
+  <si>
+    <t>*;</t>
+  </si>
+  <si>
+    <t>|;</t>
+  </si>
+  <si>
+    <t>*&amp;%;</t>
+  </si>
+  <si>
+    <t>3. Print Team/s</t>
+  </si>
+  <si>
+    <t>2. Print Teacher/s</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2072D94-46CD-413B-A0B8-272013478597}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,11 +1672,11 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1799,6 +1830,520 @@
       </c>
       <c r="B26" s="9" t="s">
         <v>38</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="56">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269E0A8F-86C6-4E77-AA5F-79422E40A562}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="N1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3" s="12"/>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="18">
+        <v>44272</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+      <c r="L8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="22"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D9" s="17">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
+      <c r="L9" s="17">
+        <v>5</v>
+      </c>
+      <c r="M9" s="23">
+        <v>-3</v>
+      </c>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="17">
+        <v>2</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="L10" s="17">
+        <v>6</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" s="17">
+        <v>3</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="L11" s="17">
+        <v>7</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="17">
+        <v>4</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="L12" s="17">
+        <v>8</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="37">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="40"/>
+      <c r="K18" s="44"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>2</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="40"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>4</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="37">
+        <v>5</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="40"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>6</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>7</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="40"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>8</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">

</xml_diff>